<commit_message>
changing format of responses given to mdx file
</commit_message>
<xml_diff>
--- a/data/starmantis.xlsx
+++ b/data/starmantis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\website\rhytididae\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\website\rhytididae\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74644D2A-1AD8-4BFA-84EA-13951067CCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484D686C-88D5-4A28-9A5A-5A3E546BD779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1694,12 +1694,12 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>46037.706946075021</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>46037.712116931143</v>
       </c>
@@ -1794,11 +1794,8 @@
       <c r="J3" t="s">
         <v>94</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>46037.740120158393</v>
       </c>
@@ -1830,7 +1827,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>46037.78267889758</v>
       </c>
@@ -1862,7 +1859,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>46037.987866882439</v>
       </c>
@@ -1894,7 +1891,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>46038.310060298092</v>
       </c>
@@ -1926,7 +1923,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>46038.800318463313</v>
       </c>
@@ -1958,7 +1955,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>46039.082558929651</v>
       </c>
@@ -1990,7 +1987,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>46039.477079865981</v>
       </c>
@@ -2022,7 +2019,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>46040.046168826717</v>
       </c>
@@ -2054,7 +2051,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>46040.649491124757</v>
       </c>
@@ -2086,7 +2083,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>46041.506417015669</v>
       </c>
@@ -2118,7 +2115,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>46041.854885037967</v>
       </c>
@@ -2150,7 +2147,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>46041.867575991208</v>
       </c>
@@ -2182,7 +2179,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>46041.892362794293</v>
       </c>
@@ -2214,7 +2211,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>46041.94871871706</v>
       </c>
@@ -2246,7 +2243,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>46041.957003748183</v>
       </c>
@@ -2278,7 +2275,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>46041.998511677302</v>
       </c>
@@ -2310,7 +2307,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>46042.019234236534</v>
       </c>
@@ -2342,7 +2339,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>46042.122229187371</v>
       </c>
@@ -2373,8 +2370,11 @@
       <c r="J21" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>46042.401316551142</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>46042.578850398597</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>46042.842304960221</v>
       </c>

</xml_diff>